<commit_message>
Updates to code to include new spawning distributions.
</commit_message>
<xml_diff>
--- a/External_data/FlowScen/FallFlows20241001_Draft.xlsx
+++ b/External_data/FlowScen/FallFlows20241001_Draft.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAF17B0-99B8-478F-8DA9-99D6336E61C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" tabRatio="876" activeTab="1" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="876" firstSheet="1" activeTab="6" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Keswick Flow Alternatives" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Scenario Description" sheetId="7" r:id="rId6"/>
     <sheet name="Shallow WRC Redds 09102024" sheetId="13" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2049,34 +2049,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="26" fillId="0" borderId="8" xfId="32" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="126" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="26" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="126" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2109,20 +2100,29 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="126" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="26" fillId="0" borderId="8" xfId="32" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="126" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="26" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="127" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="129">
@@ -9478,7 +9478,7 @@
                   <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>10000000</c:v>
@@ -11100,7 +11100,7 @@
                   <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>10000000</c:v>
@@ -27785,7 +27785,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B9A0DFFB-0EAB-4130-A4A2-055D67D97DCF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27873,7 +27873,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656674" cy="6282070"/>
+    <xdr:ext cx="8654815" cy="6274741"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -27906,7 +27906,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10821865" cy="7854462"/>
+    <xdr:ext cx="8657492" cy="6283569"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -28235,7 +28235,7 @@
   <dimension ref="A1:Q238"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L214" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="L239" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="O119" sqref="O119"/>
@@ -31458,7 +31458,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
@@ -41694,7 +41694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D67B6F-CD3E-42CC-BABC-E7E74F1F1B54}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -42067,7 +42067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75326C07-88D5-4688-9523-DFAE98186BC1}">
   <dimension ref="A1:AP71"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -42099,44 +42099,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="189" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="207" t="s">
+      <c r="B1" s="189" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="207" t="s">
+      <c r="C1" s="189" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="208" t="s">
+      <c r="D1" s="191" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="207" t="s">
+      <c r="E1" s="189" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="207" t="s">
+      <c r="F1" s="189" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="209" t="s">
+      <c r="G1" s="187" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="210" t="s">
+      <c r="H1" s="188" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="210" t="s">
+      <c r="I1" s="188" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="207" t="s">
+      <c r="J1" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="211" t="s">
+      <c r="K1" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="198" t="s">
+      <c r="N1" s="195" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="199"/>
-      <c r="P1" s="202" t="s">
+      <c r="O1" s="196"/>
+      <c r="P1" s="199" t="s">
         <v>68</v>
       </c>
       <c r="Q1" s="74">
@@ -42183,20 +42183,20 @@
       <c r="AF1" s="75"/>
     </row>
     <row r="2" spans="1:42" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="207"/>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="209"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="211"/>
-      <c r="N2" s="200"/>
-      <c r="O2" s="201"/>
-      <c r="P2" s="203"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="190"/>
+      <c r="N2" s="197"/>
+      <c r="O2" s="198"/>
+      <c r="P2" s="200"/>
       <c r="Q2" s="76">
         <v>45445</v>
       </c>
@@ -42239,34 +42239,34 @@
       <c r="AF2" s="77"/>
     </row>
     <row r="3" spans="1:42" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="207"/>
-      <c r="B3" s="207"/>
-      <c r="C3" s="207"/>
-      <c r="D3" s="208"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="209"/>
-      <c r="H3" s="210"/>
-      <c r="I3" s="210"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="211"/>
-      <c r="N3" s="204"/>
-      <c r="O3" s="205"/>
-      <c r="P3" s="206"/>
-      <c r="Q3" s="187" t="s">
+      <c r="A3" s="189"/>
+      <c r="B3" s="189"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="189"/>
+      <c r="K3" s="190"/>
+      <c r="N3" s="201"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="203"/>
+      <c r="Q3" s="204" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="188"/>
-      <c r="S3" s="188"/>
-      <c r="T3" s="188"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="188"/>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="188"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="188"/>
-      <c r="AB3" s="188"/>
+      <c r="R3" s="205"/>
+      <c r="S3" s="205"/>
+      <c r="T3" s="205"/>
+      <c r="U3" s="205"/>
+      <c r="V3" s="205"/>
+      <c r="W3" s="205"/>
+      <c r="X3" s="205"/>
+      <c r="Y3" s="205"/>
+      <c r="Z3" s="205"/>
+      <c r="AA3" s="205"/>
+      <c r="AB3" s="205"/>
       <c r="AC3" s="78"/>
       <c r="AD3" s="78"/>
       <c r="AE3" s="78"/>
@@ -42283,25 +42283,25 @@
       <c r="AP3" s="79"/>
     </row>
     <row r="4" spans="1:42" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="207"/>
-      <c r="B4" s="207"/>
-      <c r="C4" s="207"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="207"/>
-      <c r="F4" s="207"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="210"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="207"/>
-      <c r="K4" s="211"/>
+      <c r="A4" s="189"/>
+      <c r="B4" s="189"/>
+      <c r="C4" s="189"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="189"/>
+      <c r="F4" s="189"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="189"/>
+      <c r="K4" s="190"/>
       <c r="M4" s="80"/>
       <c r="N4" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="193" t="s">
+      <c r="O4" s="208" t="s">
         <v>71</v>
       </c>
-      <c r="P4" s="194"/>
+      <c r="P4" s="209"/>
       <c r="Q4" s="82">
         <v>8700</v>
       </c>
@@ -42381,10 +42381,10 @@
       <c r="N5" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="O5" s="195">
+      <c r="O5" s="210">
         <v>26</v>
       </c>
-      <c r="P5" s="196"/>
+      <c r="P5" s="211"/>
       <c r="Q5" s="99">
         <v>26</v>
       </c>
@@ -42446,10 +42446,10 @@
       <c r="N6" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="O6" s="190">
+      <c r="O6" s="193">
         <v>27</v>
       </c>
-      <c r="P6" s="197"/>
+      <c r="P6" s="194"/>
       <c r="Q6" s="108"/>
       <c r="R6" s="109">
         <v>27</v>
@@ -42515,10 +42515,10 @@
       <c r="N7" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="190">
+      <c r="O7" s="193">
         <v>23</v>
       </c>
-      <c r="P7" s="197"/>
+      <c r="P7" s="194"/>
       <c r="Q7" s="108"/>
       <c r="R7" s="109">
         <v>23</v>
@@ -42592,10 +42592,10 @@
       <c r="N8" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="O8" s="190">
+      <c r="O8" s="193">
         <v>13</v>
       </c>
-      <c r="P8" s="197"/>
+      <c r="P8" s="194"/>
       <c r="Q8" s="108"/>
       <c r="R8" s="110"/>
       <c r="S8" s="109">
@@ -42669,10 +42669,10 @@
       <c r="N9" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="190">
+      <c r="O9" s="193">
         <v>22</v>
       </c>
-      <c r="P9" s="197"/>
+      <c r="P9" s="194"/>
       <c r="Q9" s="108"/>
       <c r="R9" s="110"/>
       <c r="S9" s="119">
@@ -42744,10 +42744,10 @@
       <c r="N10" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="O10" s="190">
+      <c r="O10" s="193">
         <v>10</v>
       </c>
-      <c r="P10" s="197"/>
+      <c r="P10" s="194"/>
       <c r="Q10" s="108"/>
       <c r="R10" s="110"/>
       <c r="S10" s="119">
@@ -42821,10 +42821,10 @@
       <c r="N11" s="98" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="189">
+      <c r="O11" s="192">
         <v>23</v>
       </c>
-      <c r="P11" s="190"/>
+      <c r="P11" s="193"/>
       <c r="Q11" s="108"/>
       <c r="R11" s="110"/>
       <c r="S11" s="110"/>
@@ -42898,10 +42898,10 @@
       <c r="N12" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="O12" s="189">
+      <c r="O12" s="192">
         <v>34</v>
       </c>
-      <c r="P12" s="190"/>
+      <c r="P12" s="193"/>
       <c r="Q12" s="108"/>
       <c r="R12" s="110"/>
       <c r="S12" s="110"/>
@@ -42975,10 +42975,10 @@
       <c r="N13" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="O13" s="189">
+      <c r="O13" s="192">
         <v>26</v>
       </c>
-      <c r="P13" s="190"/>
+      <c r="P13" s="193"/>
       <c r="Q13" s="108"/>
       <c r="R13" s="110"/>
       <c r="S13" s="110"/>
@@ -43052,10 +43052,10 @@
       <c r="N14" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="O14" s="189">
+      <c r="O14" s="192">
         <v>25</v>
       </c>
-      <c r="P14" s="190"/>
+      <c r="P14" s="193"/>
       <c r="Q14" s="108"/>
       <c r="R14" s="110"/>
       <c r="S14" s="110"/>
@@ -43127,10 +43127,10 @@
       <c r="N15" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="O15" s="189">
+      <c r="O15" s="192">
         <v>27</v>
       </c>
-      <c r="P15" s="190"/>
+      <c r="P15" s="193"/>
       <c r="Q15" s="108"/>
       <c r="R15" s="110"/>
       <c r="S15" s="110"/>
@@ -43204,10 +43204,10 @@
       <c r="N16" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="O16" s="189">
+      <c r="O16" s="192">
         <v>18</v>
       </c>
-      <c r="P16" s="190"/>
+      <c r="P16" s="193"/>
       <c r="Q16" s="108"/>
       <c r="R16" s="110"/>
       <c r="S16" s="110"/>
@@ -43281,10 +43281,10 @@
       <c r="N17" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="O17" s="189">
+      <c r="O17" s="192">
         <v>34</v>
       </c>
-      <c r="P17" s="190"/>
+      <c r="P17" s="193"/>
       <c r="Q17" s="108"/>
       <c r="R17" s="110"/>
       <c r="S17" s="110"/>
@@ -43350,10 +43350,10 @@
       <c r="N18" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="O18" s="189">
+      <c r="O18" s="192">
         <v>14</v>
       </c>
-      <c r="P18" s="190"/>
+      <c r="P18" s="193"/>
       <c r="Q18" s="108"/>
       <c r="R18" s="110"/>
       <c r="S18" s="110"/>
@@ -43425,10 +43425,10 @@
       <c r="N19" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="189">
+      <c r="O19" s="192">
         <v>16</v>
       </c>
-      <c r="P19" s="190"/>
+      <c r="P19" s="193"/>
       <c r="Q19" s="108"/>
       <c r="R19" s="110"/>
       <c r="S19" s="110"/>
@@ -43500,10 +43500,10 @@
       <c r="N20" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="O20" s="189">
+      <c r="O20" s="192">
         <v>24</v>
       </c>
-      <c r="P20" s="190"/>
+      <c r="P20" s="193"/>
       <c r="Q20" s="108"/>
       <c r="R20" s="110"/>
       <c r="S20" s="110"/>
@@ -43571,10 +43571,10 @@
       <c r="N21" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="O21" s="189">
+      <c r="O21" s="192">
         <v>23</v>
       </c>
-      <c r="P21" s="190"/>
+      <c r="P21" s="193"/>
       <c r="Q21" s="108"/>
       <c r="R21" s="110"/>
       <c r="S21" s="110"/>
@@ -43618,8 +43618,8 @@
       <c r="L22" s="127"/>
       <c r="M22" s="97"/>
       <c r="N22" s="98"/>
-      <c r="O22" s="189"/>
-      <c r="P22" s="190"/>
+      <c r="O22" s="192"/>
+      <c r="P22" s="193"/>
       <c r="Q22" s="108"/>
       <c r="R22" s="110"/>
       <c r="S22" s="110"/>
@@ -43651,8 +43651,8 @@
       <c r="L23" s="127"/>
       <c r="M23" s="97"/>
       <c r="N23" s="98"/>
-      <c r="O23" s="189"/>
-      <c r="P23" s="190"/>
+      <c r="O23" s="192"/>
+      <c r="P23" s="193"/>
       <c r="Q23" s="108"/>
       <c r="R23" s="110"/>
       <c r="S23" s="110"/>
@@ -43684,8 +43684,8 @@
       <c r="L24" s="127"/>
       <c r="M24" s="97"/>
       <c r="N24" s="98"/>
-      <c r="O24" s="189"/>
-      <c r="P24" s="190"/>
+      <c r="O24" s="192"/>
+      <c r="P24" s="193"/>
       <c r="Q24" s="108"/>
       <c r="R24" s="110"/>
       <c r="S24" s="110"/>
@@ -43717,8 +43717,8 @@
       <c r="L25" s="127"/>
       <c r="M25" s="97"/>
       <c r="N25" s="98"/>
-      <c r="O25" s="189"/>
-      <c r="P25" s="190"/>
+      <c r="O25" s="192"/>
+      <c r="P25" s="193"/>
       <c r="Q25" s="108"/>
       <c r="R25" s="110"/>
       <c r="S25" s="110"/>
@@ -43750,8 +43750,8 @@
       <c r="L26" s="127"/>
       <c r="M26" s="129"/>
       <c r="N26" s="130"/>
-      <c r="O26" s="191"/>
-      <c r="P26" s="192"/>
+      <c r="O26" s="206"/>
+      <c r="P26" s="207"/>
       <c r="Q26" s="131"/>
       <c r="R26" s="132"/>
       <c r="S26" s="132"/>
@@ -45254,28 +45254,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="K1:K4"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
     <mergeCell ref="Q3:AB3"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="O26:P26"/>
@@ -45292,6 +45270,28 @@
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="K1:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="L1:L1048576">
     <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">

</xml_diff>